<commit_message>
carpetas faltantes para repositorio completo
</commit_message>
<xml_diff>
--- a/archivos/tabla_presupuesto.xlsx
+++ b/archivos/tabla_presupuesto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESTADISTICA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.10.18.128\info\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08B32CE-834B-46D3-A46F-22EFFBD372D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4097B6-16FC-4193-8E4F-FA14C49A2ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-735" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1140,7 +1140,7 @@
     <t>2625</t>
   </si>
   <si>
-    <t>CHERRY_TESSINO</t>
+    <t>CHERRY TESSINO</t>
   </si>
 </sst>
 </file>
@@ -1199,18 +1199,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1489,8 +1478,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:S1172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1151" workbookViewId="0">
+      <selection activeCell="C1172" sqref="C1172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>